<commit_message>
modelo de classificação de equipamentos
</commit_message>
<xml_diff>
--- a/documents/teste_modelo.xlsx
+++ b/documents/teste_modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\chatbot_hipotese\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF7D759-A18D-4FBB-A5A2-DDF4652C432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5E56B1-719C-45DF-BA03-8F40FC205CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C4CE6E0E-49B7-4497-A931-1021F84E34DD}"/>
   </bookViews>
@@ -34,162 +34,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
-  <si>
-    <t>- A bomba está fazendo barulho excessivo e vibrando muito.</t>
-  </si>
-  <si>
-    <t>- A bomba não está ligando quando o sistema é ativado.</t>
-  </si>
-  <si>
-    <t>- A bomba está apresentando vazamento de água.</t>
-  </si>
-  <si>
-    <t>- A bomba está funcionando com baixo desempenho.</t>
-  </si>
-  <si>
-    <t>- A bomba está superaquecendo e desligando automaticamente.</t>
-  </si>
-  <si>
-    <t>- O rolamento está emitindo ruídos estranhos quando girado.</t>
-  </si>
-  <si>
-    <t>- O rolamento está travando, impedindo o movimento suave da máquina.</t>
-  </si>
-  <si>
-    <t>- O rolamento está apresentando folga excessiva.</t>
-  </si>
-  <si>
-    <t>- O rolamento está superaquecendo, indicando possível falta de lubrificação.</t>
-  </si>
-  <si>
-    <t>- O rolamento está desgastado e precisa ser substituído.</t>
-  </si>
-  <si>
-    <t>- A válvula está vazando mesmo quando fechada.</t>
-  </si>
-  <si>
-    <t>- A válvula está emperrada e não consegue abrir ou fechar corretamente.</t>
-  </si>
-  <si>
-    <t>- A válvula está apresentando fluxo irregular.</t>
-  </si>
-  <si>
-    <t>- A válvula está com dificuldade para ser acionada manualmente.</t>
-  </si>
-  <si>
-    <t>- A válvula está apresentando corrosão e desgaste.</t>
-  </si>
-  <si>
-    <t>- A corrente está solta e escapando das engrenagens.</t>
-  </si>
-  <si>
-    <t>- O acionamento por corrente está fazendo barulho de atrito metálico.</t>
-  </si>
-  <si>
-    <t>- A corrente está desalinhada, causando mau funcionamento do sistema.</t>
-  </si>
-  <si>
-    <t>- O acionamento por corrente está se desgastando rapidamente.</t>
-  </si>
-  <si>
-    <t>- A corrente está quebrando com frequência.</t>
-  </si>
-  <si>
-    <t>- A caixa de engrenagens está fazendo ruídos de engrenagens rangendo.</t>
-  </si>
-  <si>
-    <t>- A caixa de engrenagens está superaquecendo, indicando atrito excessivo.</t>
-  </si>
-  <si>
-    <t>- A caixa de engrenagens está apresentando vazamentos de óleo lubrificante.</t>
-  </si>
-  <si>
-    <t>- A caixa de engrenagens está com engrenagens desgastadas.</t>
-  </si>
-  <si>
-    <t>- A caixa de engrenagens está travando, impedindo o movimento suave do sistema.</t>
-  </si>
-  <si>
-    <t>- O reservatório de óleo está vazando.</t>
-  </si>
-  <si>
-    <t>- A bomba de óleo não está funcionando adequadamente.</t>
-  </si>
-  <si>
-    <t>- O filtro de óleo está obstruído.</t>
-  </si>
-  <si>
-    <t>- O radiador de óleo está com mau funcionamento.</t>
-  </si>
-  <si>
-    <t>- O sensor de óleo está com defeito.</t>
-  </si>
-  <si>
-    <t>- As polias em V estão desgastadas.</t>
-  </si>
-  <si>
-    <t>- A correia em V está frouxa.</t>
-  </si>
-  <si>
-    <t>- Os tensionadores em V estão com defeito.</t>
-  </si>
-  <si>
-    <t>- O acoplamento em V está com mau funcionamento.</t>
-  </si>
-  <si>
-    <t>- O sistema de acionamento por correia em V está desalinhado.</t>
-  </si>
-  <si>
-    <t>- O ventilador está com ruído excessivo.</t>
-  </si>
-  <si>
-    <t>- O exaustor não está funcionando.</t>
-  </si>
-  <si>
-    <t>- O soprador está com baixo fluxo de ar.</t>
-  </si>
-  <si>
-    <t>- O sistema de ventiladores está superaquecendo.</t>
-  </si>
-  <si>
-    <t>- O ventilador está com mau funcionamento elétrico.</t>
-  </si>
-  <si>
-    <t>- O purgador de vapor está vazando.</t>
-  </si>
-  <si>
-    <t>- O purgador de vapor não está liberando condensado corretamente.</t>
-  </si>
-  <si>
-    <t>- O purgador de vapor está com obstrução.</t>
-  </si>
-  <si>
-    <t>- O purgador de vapor está emitindo vapor excessivo.</t>
-  </si>
-  <si>
-    <t>- O purgador de vapor está com mau funcionamento mecânico.</t>
-  </si>
-  <si>
-    <t>- O motor elétrico não está ligando.</t>
-  </si>
-  <si>
-    <t>- O motor elétrico está superaquecendo.</t>
-  </si>
-  <si>
-    <t>- O motor elétrico está emitindo cheiro de queimado.</t>
-  </si>
-  <si>
-    <t>- O motor elétrico está apresentando falha intermitente.</t>
-  </si>
-  <si>
-    <t>- O motor elétrico está consumindo mais energia do que o normal.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>classe</t>
   </si>
   <si>
     <t>exemplos</t>
+  </si>
+  <si>
+    <t>A bomba está apresentando baixa pressão de saída.</t>
+  </si>
+  <si>
+    <t>A bomba está consumindo energia em excesso.</t>
+  </si>
+  <si>
+    <t>A bomba está apresentando desgaste prematuro das pás.</t>
+  </si>
+  <si>
+    <t>A bomba está com dificuldade de partir.</t>
+  </si>
+  <si>
+    <t>A bomba está produzindo vibrações anormais.</t>
+  </si>
+  <si>
+    <t>O rolamento está superaquecendo rapidamente.</t>
+  </si>
+  <si>
+    <t>O rolamento está com sinais de desalinhamento.</t>
+  </si>
+  <si>
+    <t>O rolamento está apresentando corrosão.</t>
+  </si>
+  <si>
+    <t>O rolamento está com folga axial excessiva.</t>
+  </si>
+  <si>
+    <t>O rolamento está produzindo ruídos de rangido.</t>
+  </si>
+  <si>
+    <t>A válvula está abrindo ou fechando lentamente.</t>
+  </si>
+  <si>
+    <t>A válvula está apresentando vazamentos externos.</t>
+  </si>
+  <si>
+    <t>A válvula está com dificuldade de manter a posição.</t>
+  </si>
+  <si>
+    <t>A válvula está com dificuldade de realizar o corte.</t>
+  </si>
+  <si>
+    <t>A válvula está apresentando falha no atuador.</t>
+  </si>
+  <si>
+    <t>A corrente está escapando do conjunto de engrenagens.</t>
+  </si>
+  <si>
+    <t>O acionamento por corrente está perdendo tensão.</t>
+  </si>
+  <si>
+    <t>A corrente está apresentando desgaste excessivo.</t>
+  </si>
+  <si>
+    <t>O acionamento por corrente está produzindo ruídos.</t>
+  </si>
+  <si>
+    <t>A corrente está quebrando com frequência.</t>
+  </si>
+  <si>
+    <t>A caixa de engrenagens está com desalinhamento.</t>
+  </si>
+  <si>
+    <t>A caixa de engrenagens está com vazamentos de óleo.</t>
+  </si>
+  <si>
+    <t>A caixa de engrenagens está com ruídos de atrito.</t>
+  </si>
+  <si>
+    <t>A caixa de engrenagens está com engrenagens gastas.</t>
+  </si>
+  <si>
+    <t>A caixa de engrenagens está travando durante operação.</t>
+  </si>
+  <si>
+    <t>O reservatório de óleo está com nível baixo.</t>
+  </si>
+  <si>
+    <t>A bomba de óleo está com mau funcionamento.</t>
+  </si>
+  <si>
+    <t>O filtro de óleo está obstruído e precisa ser substituído.</t>
+  </si>
+  <si>
+    <t>O radiador de óleo está com vazamentos.</t>
+  </si>
+  <si>
+    <t>O sensor de óleo está com falha na leitura.</t>
+  </si>
+  <si>
+    <t>As polias em V estão desalinhadas e causando desgaste.</t>
+  </si>
+  <si>
+    <t>A correia em V está solta e precisa ser tensionada.</t>
+  </si>
+  <si>
+    <t>Os tensionadores em V estão com ruídos.</t>
+  </si>
+  <si>
+    <t>O acoplamento em V está com desgaste excessivo.</t>
+  </si>
+  <si>
+    <t>O ventilador está com baixo fluxo de ar.</t>
+  </si>
+  <si>
+    <t>O exaustor está produzindo ruídos anormais.</t>
+  </si>
+  <si>
+    <t>O ventilador está com desequilíbrio nas pás.</t>
+  </si>
+  <si>
+    <t>O ventilador está superaquecendo.</t>
+  </si>
+  <si>
+    <t>O exaustor está com falha no motor.</t>
+  </si>
+  <si>
+    <t>O purgador de vapor está com vazamentos.</t>
+  </si>
+  <si>
+    <t>O purgador de vapor não está liberando condensado.</t>
+  </si>
+  <si>
+    <t>O purgador de vapor está com operação intermitente.</t>
+  </si>
+  <si>
+    <t>O purgador de vapor está obstruído.</t>
+  </si>
+  <si>
+    <t>O purgador de vapor está produzindo ruídos.</t>
+  </si>
+  <si>
+    <t>O motor elétrico está superaquecendo.</t>
+  </si>
+  <si>
+    <t>O motor elétrico está com mau contato nos terminais.</t>
+  </si>
+  <si>
+    <t>O motor elétrico está com falha no rotor.</t>
+  </si>
+  <si>
+    <t>O motor elétrico está produzindo ruídos anormais.</t>
+  </si>
+  <si>
+    <t>O motor elétrico está com perda de potência.</t>
   </si>
 </sst>
 </file>
@@ -561,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1AD7CC-E1EE-47B8-B589-819C571C9B06}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,282 +572,282 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -858,39 +855,39 @@
         <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,39 +895,39 @@
         <v>8</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -938,47 +935,39 @@
         <v>9</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>10</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>